<commit_message>
fix: Commit correct results
</commit_message>
<xml_diff>
--- a/data-labs.xlsx
+++ b/data-labs.xlsx
@@ -240,7 +240,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -365,61 +365,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>403191083</c:v>
+                  <c:v>93036641</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>389770642</c:v>
+                  <c:v>94252564</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>390833287</c:v>
+                  <c:v>94446894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>391485273</c:v>
+                  <c:v>94646841</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>395506067</c:v>
+                  <c:v>94847369</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>417645533</c:v>
+                  <c:v>99318001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>433453742</c:v>
+                  <c:v>101212711</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>424760256</c:v>
+                  <c:v>102346371</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>469804696</c:v>
+                  <c:v>108746940</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>501025778</c:v>
+                  <c:v>120074375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>510410833</c:v>
+                  <c:v>121873852</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>523819601</c:v>
+                  <c:v>122391716</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>527124132</c:v>
+                  <c:v>123048072</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>637479910</c:v>
+                  <c:v>128920942</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1084335689</c:v>
+                  <c:v>192796323</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1431523285</c:v>
+                  <c:v>265876588</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1470617405</c:v>
+                  <c:v>294861979</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1496208562</c:v>
+                  <c:v>304664490</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1526494797</c:v>
+                  <c:v>311390564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -434,11 +434,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="46702210"/>
-        <c:axId val="23802047"/>
+        <c:axId val="51508554"/>
+        <c:axId val="51853001"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46702210"/>
+        <c:axId val="51508554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +466,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23802047"/>
+        <c:crossAx val="51853001"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -474,7 +474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23802047"/>
+        <c:axId val="51853001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +511,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46702210"/>
+        <c:crossAx val="51508554"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -559,7 +559,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -684,61 +684,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>51465464</c:v>
+                  <c:v>51442187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47346008</c:v>
+                  <c:v>47049680</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42290326</c:v>
+                  <c:v>43121466</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42330258</c:v>
+                  <c:v>42999716</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42678065</c:v>
+                  <c:v>43314530</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66194385</c:v>
+                  <c:v>64611869</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70839735</c:v>
+                  <c:v>68278414</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67937775</c:v>
+                  <c:v>68768311</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78558199</c:v>
+                  <c:v>80729080</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99939500</c:v>
+                  <c:v>103031369</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103987612</c:v>
+                  <c:v>110832062</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>104983765</c:v>
+                  <c:v>114464165</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104756394</c:v>
+                  <c:v>116422450</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>134649234</c:v>
+                  <c:v>124861673</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>247970010</c:v>
+                  <c:v>249150229</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>324749792</c:v>
+                  <c:v>377067302</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>356913514</c:v>
+                  <c:v>353532543</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>381081550</c:v>
+                  <c:v>360349328</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>379304607</c:v>
+                  <c:v>373602684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -753,11 +753,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="50821172"/>
-        <c:axId val="62770314"/>
+        <c:axId val="55140130"/>
+        <c:axId val="97036170"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50821172"/>
+        <c:axId val="55140130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +785,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62770314"/>
+        <c:crossAx val="97036170"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -793,7 +793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62770314"/>
+        <c:axId val="97036170"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +830,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50821172"/>
+        <c:crossAx val="55140130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -951,7 +951,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B20"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -975,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>51465464</v>
+        <v>51442187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>47346008</v>
+        <v>47049680</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>42290326</v>
+        <v>43121466</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>42330258</v>
+        <v>42999716</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>42678065</v>
+        <v>43314530</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>66194385</v>
+        <v>64611869</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>70839735</v>
+        <v>68278414</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>67937775</v>
+        <v>68768311</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>78558199</v>
+        <v>80729080</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>99939500</v>
+        <v>103031369</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,7 +1055,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>103987612</v>
+        <v>110832062</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,7 +1063,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>104983765</v>
+        <v>114464165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>104756394</v>
+        <v>116422450</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>134649234</v>
+        <v>124861673</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,7 +1087,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>247970010</v>
+        <v>249150229</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,7 +1095,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>324749792</v>
+        <v>377067302</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1103,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>356913514</v>
+        <v>353532543</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1111,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>381081550</v>
+        <v>360349328</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,7 +1119,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>379304607</v>
+        <v>373602684</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>403191083</v>
+        <v>93036641</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>389770642</v>
+        <v>94252564</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,7 +1143,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>390833287</v>
+        <v>94446894</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>391485273</v>
+        <v>94646841</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,7 +1159,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>395506067</v>
+        <v>94847369</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>417645533</v>
+        <v>99318001</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1175,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>433453742</v>
+        <v>101212711</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>424760256</v>
+        <v>102346371</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>469804696</v>
+        <v>108746940</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>501025778</v>
+        <v>120074375</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1207,7 +1207,7 @@
         <v>12</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>510410833</v>
+        <v>121873852</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1215,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>523819601</v>
+        <v>122391716</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>527124132</v>
+        <v>123048072</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,7 +1231,7 @@
         <v>15</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>637479910</v>
+        <v>128920942</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1239,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1084335689</v>
+        <v>192796323</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1247,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1431523285</v>
+        <v>265876588</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,7 +1255,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1470617405</v>
+        <v>294861979</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,7 +1263,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1496208562</v>
+        <v>304664490</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,7 +1271,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1526494797</v>
+        <v>311390564</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1294,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:B20 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B23:B41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>